<commit_message>
toolbar works + premier league table file created
</commit_message>
<xml_diff>
--- a/gui/mecze.xlsx
+++ b/gui/mecze.xlsx
@@ -494,37 +494,33 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Finished</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Leeds</t>
+          <t>Wolves</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/lvs4WW5k-d2cNSxrp.png</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>3-1</t>
-        </is>
-      </c>
+          <t>https://www.flashscore.com/res/image/data/OMUzjDkC-rawILjE1.png</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/v3SzDxVH-EwpAw8YN.png</t>
+          <t>https://www.flashscore.com/res/image/data/G0q9xjRq-IccPlIAs.png</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Tottenham</t>
+          <t>Brighton</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>ENDED</t>
+          <t>SCHEDULED</t>
         </is>
       </c>
     </row>
@@ -542,37 +538,33 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Finished</t>
+          <t>15:05</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Sheffield Utd</t>
+          <t>Aston Villa</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/8nXNvlA6-OWyZW5TC.png</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>0-2</t>
-        </is>
-      </c>
+          <t>https://www.flashscore.com/res/image/data/UHchCEVH-jm1Xyzp7.png</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/GfkvlLmC-6sMoYuga.png</t>
+          <t>https://www.flashscore.com/res/image/data/GhGV3qjT-rBodzytr.png</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Crystal Palace</t>
+          <t>Manchester Utd</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>ENDED</t>
+          <t>SCHEDULED</t>
         </is>
       </c>
     </row>
@@ -590,38 +582,33 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>44  min</t>
+          <t>17:30</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>GOAL
-Manchester City</t>
+          <t>West Ham</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/0vgscFU0-zZRehMhm.png</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>1-0</t>
-        </is>
-      </c>
+          <t>https://www.flashscore.com/res/image/data/YeSfKGlC-hrtlQ906.png</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/lMxEQ8me-2B0QucIK.png</t>
+          <t>https://www.flashscore.com/res/image/data/EBfZuwme-Onr593up.png</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Chelsea</t>
+          <t>Everton</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>LIVE</t>
+          <t>SCHEDULED</t>
         </is>
       </c>
     </row>
@@ -639,28 +626,28 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>21:15</t>
+          <t>20:00</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Arsenal</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/x82JgBjC-2B0QucIK.png</t>
+          <t>https://www.flashscore.com/res/image/data/0n1ffK6k-pU2IsJm8.png</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/2VvVDtSq-Ozt88U7U.png</t>
+          <t>https://www.flashscore.com/res/image/data/QsGXnZjC-hUScfdXD.png</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Southampton</t>
+          <t>West Brom</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -683,37 +670,33 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Finished</t>
+          <t>13:00</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Nantes</t>
+          <t>St Etienne</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/vTVURLne-nsw9tAch.png</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>3-0</t>
-        </is>
-      </c>
+          <t>https://www.flashscore.com/res/image/data/MF4bIRPq-Qk1sBuEM.png</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/QVabyUVH-2Fz8tP17.png</t>
+          <t>https://www.flashscore.com/res/image/data/t6Kb5X76-Qk1sBuEM.png</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Bordeaux</t>
+          <t>Marseille</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>ENDED</t>
+          <t>SCHEDULED</t>
         </is>
       </c>
     </row>
@@ -731,37 +714,33 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Finished</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Lyon</t>
+          <t>Angers</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/bkuX6RS0-IRbzmzRB.png</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>4-1</t>
-        </is>
-      </c>
+          <t>https://www.flashscore.com/res/image/data/IN9Ib7jT-EorrQF3M.png</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/0r9EzUS0-6knD5Jyp.png</t>
+          <t>https://www.flashscore.com/res/image/data/IVjOpykC-YHD0XcTg.png</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Lorient</t>
+          <t>Dijon</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>ENDED</t>
+          <t>SCHEDULED</t>
         </is>
       </c>
     </row>
@@ -774,42 +753,38 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>GERMANY - Bundesliga</t>
+          <t>FRANCE - Ligue 1</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Finished</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Dortmund</t>
+          <t>Metz</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/xSfDCO76-dhhpTYj5.png</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>3-2</t>
-        </is>
-      </c>
+          <t>https://www.flashscore.com/res/image/data/SCdF7fjT-4pdbha5J.png</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/fNS5fTmC-hK7y9vIK.png</t>
+          <t>https://www.flashscore.com/res/image/data/xtTjGRT0-Sr136dyl.png</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>RB Leipzig</t>
+          <t>Nimes</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>ENDED</t>
+          <t>SCHEDULED</t>
         </is>
       </c>
     </row>
@@ -822,42 +797,38 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>GERMANY - Bundesliga</t>
+          <t>FRANCE - Ligue 1</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Finished</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Hoffenheim</t>
+          <t>Nice</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/IyZBMF7k-6cGmlIiN.png</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>4-2</t>
-        </is>
-      </c>
+          <t>https://www.flashscore.com/res/image/data/bJCGymle-jiROSmFn.png</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/jy0u6bgT-I1gtUEya.png</t>
+          <t>https://www.flashscore.com/res/image/data/lWu2w4ne-fXJWG6Mg.png</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Schalke</t>
+          <t>Brest</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>ENDED</t>
+          <t>SCHEDULED</t>
         </is>
       </c>
     </row>
@@ -870,42 +841,38 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>GERMANY - Bundesliga</t>
+          <t>FRANCE - Ligue 1</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Finished</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Strasbourg</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/pIavfLS0-C6khRCLH.png</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>0-0</t>
-        </is>
-      </c>
+          <t>https://www.flashscore.com/res/image/data/2XOhzSQq-4SOLY7oe.png</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/dWZYQIPq-YFjlSh6B.png</t>
+          <t>https://www.flashscore.com/res/image/data/U3fC5I96-EkChIdLk.png</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Bayer Leverkusen</t>
+          <t>Montpellier</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>ENDED</t>
+          <t>SCHEDULED</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Button for refrashing matches
</commit_message>
<xml_diff>
--- a/gui/mecze.xlsx
+++ b/gui/mecze.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,33 +494,37 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>Finished</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Wolves</t>
+          <t>Burnley</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/OMUzjDkC-rawILjE1.png</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
+          <t>https://www.flashscore.com/res/image/data/MLYdfXhT-vajdyYuI.png</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0-4</t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/G0q9xjRq-IccPlIAs.png</t>
+          <t>https://www.flashscore.com/res/image/data/lvs4WW5k-d2cNSxrp.png</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Brighton</t>
+          <t>Leeds</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>SCHEDULED</t>
+          <t>ENDED</t>
         </is>
       </c>
     </row>
@@ -538,33 +542,37 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>15:05</t>
+          <t>67  min</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Aston Villa</t>
+          <t>Southampton</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/UHchCEVH-jm1Xyzp7.png</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
+          <t>https://www.flashscore.com/res/image/data/2VvVDtSq-Ozt88U7U.png</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2-0</t>
+        </is>
+      </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/GhGV3qjT-rBodzytr.png</t>
+          <t>https://www.flashscore.com/res/image/data/fkbYUWme-fcuGVCfD.png</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Manchester Utd</t>
+          <t>Fulham</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>SCHEDULED</t>
+          <t>LIVE</t>
         </is>
       </c>
     </row>
@@ -582,28 +590,28 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>17:30</t>
+          <t>21:00</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>West Ham</t>
+          <t>Brighton</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/YeSfKGlC-hrtlQ906.png</t>
+          <t>https://www.flashscore.com/res/image/data/G0q9xjRq-IccPlIAs.png</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/EBfZuwme-Onr593up.png</t>
+          <t>https://www.flashscore.com/res/image/data/YeSfKGlC-hrtlQ906.png</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Everton</t>
+          <t>West Ham</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -621,38 +629,42 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ENGLAND - Premier League</t>
+          <t>GERMANY - Bundesliga</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>20:00</t>
+          <t>Finished</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Arsenal</t>
+          <t>Arminia Bielefeld</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/0n1ffK6k-pU2IsJm8.png</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr"/>
+          <t>https://www.flashscore.com/res/image/data/tbqzXYS0-6XlDe17l.png</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>1-1</t>
+        </is>
+      </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/QsGXnZjC-hUScfdXD.png</t>
+          <t>https://www.flashscore.com/res/image/data/IyZBMF7k-6cGmlIiN.png</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>West Brom</t>
+          <t>Hoffenheim</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>SCHEDULED</t>
+          <t>ENDED</t>
         </is>
       </c>
     </row>
@@ -665,38 +677,42 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>FRANCE - Ligue 1</t>
+          <t>GERMANY - Bundesliga</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>Finished</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>St Etienne</t>
+          <t>Augsburg</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/MF4bIRPq-Qk1sBuEM.png</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr"/>
+          <t>https://www.flashscore.com/res/image/data/Qgbz4piC-tGGTvWkH.png</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2-0</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/t6Kb5X76-Qk1sBuEM.png</t>
+          <t>https://www.flashscore.com/res/image/data/pIavfLS0-C6khRCLH.png</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Marseille</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>SCHEDULED</t>
+          <t>ENDED</t>
         </is>
       </c>
     </row>
@@ -709,38 +725,42 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>FRANCE - Ligue 1</t>
+          <t>GERMANY - Bundesliga</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>Finished</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Angers</t>
+          <t>B. Monchengladbach</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/IN9Ib7jT-EorrQF3M.png</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr"/>
+          <t>https://www.flashscore.com/res/image/data/tjlAHwhT-xQEMKj97.png</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>1-2</t>
+        </is>
+      </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/IVjOpykC-YHD0XcTg.png</t>
+          <t>https://www.flashscore.com/res/image/data/fgQWGn86-Gp7OHZN8.png</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Dijon</t>
+          <t>Stuttgart</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>SCHEDULED</t>
+          <t>ENDED</t>
         </is>
       </c>
     </row>
@@ -753,38 +773,42 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>FRANCE - Ligue 1</t>
+          <t>GERMANY - Bundesliga</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>Finished</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Metz</t>
+          <t>Bayer Leverkusen</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/SCdF7fjT-4pdbha5J.png</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr"/>
+          <t>https://www.flashscore.com/res/image/data/dWZYQIPq-YFjlSh6B.png</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>1-1</t>
+        </is>
+      </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/xtTjGRT0-Sr136dyl.png</t>
+          <t>https://www.flashscore.com/res/image/data/0OMJUule-4O0wvXLr.png</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Nimes</t>
+          <t>Union Berlin</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>SCHEDULED</t>
+          <t>ENDED</t>
         </is>
       </c>
     </row>
@@ -797,38 +821,42 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>FRANCE - Ligue 1</t>
+          <t>GERMANY - Bundesliga</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>Finished</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Nice</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/bJCGymle-jiROSmFn.png</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr"/>
+          <t>https://www.flashscore.com/res/image/data/0pdxCFiT-jcldQWzO.png</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>2-2</t>
+        </is>
+      </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/lWu2w4ne-fXJWG6Mg.png</t>
+          <t>https://www.flashscore.com/res/image/data/lWGBVoA6-88qkLtMj.png</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Brest</t>
+          <t>Bayern Munich</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>SCHEDULED</t>
+          <t>ENDED</t>
         </is>
       </c>
     </row>
@@ -841,36 +869,1957 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>FRANCE - Ligue 1</t>
+          <t>GERMANY - Bundesliga</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>Finished</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Strasbourg</t>
+          <t>Hertha Berlin</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/2XOhzSQq-4SOLY7oe.png</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr"/>
+          <t>https://www.flashscore.com/res/image/data/j1FIuRAN-C6khRCLH.png</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0-0</t>
+        </is>
+      </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>https://www.flashscore.com/res/image/data/U3fC5I96-EkChIdLk.png</t>
+          <t>https://www.flashscore.com/res/image/data/KMphsCCN-Umm0PjjU.png</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Montpellier</t>
+          <t>FC Koln</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>GERMANY - Bundesliga</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Finished</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Schalke</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/jy0u6bgT-I1gtUEya.png</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>4-3</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/2aegVtQq-h85SGgwF.png</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Eintracht Frankfurt</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>11</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>ITALY - Serie A</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Finished</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Genoa</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/Szt5ATne-ERLRjHRE.png</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>3-4</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/z3aHqFBN-S82PeYBB.png</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Atalanta</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>12</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>ITALY - Serie A</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Finished</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Spezia</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/08qns8VH-pI6ga41n.png</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>4-1</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/dhGobOA6-j3aMQhBo.png</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Torino</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>13</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>ITALY - Serie A</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Juventus</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/xxLGMOlC-QPFkwCmU.png</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/Y9Dpez96-dYTmixLI.png</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Inter</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>SCHEDULED</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>14</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>ITALY - Serie A</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>20:45</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>AS Roma</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/j31Z1pne-Oh9bbJkf.png</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/4CLpo27k-67BxS1ca.png</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Lazio</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>SCHEDULED</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>15</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>NETHERLANDS - Eredivisie - Relegation - Play Offs</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Half Time min</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Breda</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/0fqlZvA6-C0SKTTat.png</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>1-0</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/8tDUPO86-4CAMmnBj.png</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>FC Volendam</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>LIVE</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>16</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>NETHERLANDS - Eredivisie - Relegation - Play Offs</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>18:45</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Graafschap</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/M52434oe-vFG942fq.png</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/z5aqbrkC-8lF1ED0e.png</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Roda</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>SCHEDULED</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>17</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>NETHERLANDS - Eredivisie - Relegation - Play Offs</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Almere City</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/xGubPZ7k-dOhw1vK4.png</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/C8FCtESq-xUnkdXKi.png</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Nijmegen</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>SCHEDULED</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>18</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>AFRICA - CAF Champions League - Play Offs</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>CR Belouizdad</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/0Occ50UH-6kSyv7Al.png</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/MwJ5a4AN-zas0t51T.png</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Esperance Tunis</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>SCHEDULED</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>19</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>AFRICA - CAF Champions League - Play Offs</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Kaizer Chiefs</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/6wU1xTiT-tWfupjVk.png</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/bqLBByT0-tbol2YzC.png</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Simba</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>SCHEDULED</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>20</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>AFRICA - CAF Champions League - Play Offs</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Al Ahly</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/jPMoEDoe-OtFRdJts.png</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/tOpnxPoe-KCzkP6EJ.png</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Mamelodi Sundowns</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>SCHEDULED</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>21</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>ALBANIA - First Division - Promotion Group</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Finished</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Besa Kavaje</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/Qae6QJRq-4UonyDdt.png</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>2-4</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/U1UHfgU0-dp4XfiFp.png</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Tomori Berat</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>22</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>ALBANIA - First Division - Promotion Group</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Finished</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Burreli</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/4bLPEF86-ttSkQ5rb.png</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>2-1</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/2kckHG96-4Mqz9cCl.png</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Dinamo Tirana</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>23</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>ALBANIA - First Division - Promotion Group</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Finished</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Egnatia Rrogozhine</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/CzPXaD96-MaHtbDtj.png</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>4-2</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/WW1DqOlC-8IvC3XvS.png</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Pogradeci</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>24</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>ALBANIA - First Division - Promotion Group</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Finished</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Vora</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/8dBqaBWH-SdI2r7on.png</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>1-5</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/Ct7R8T76-6yRdKGi3.png</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Korabi Peshkopi</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>25</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>ALBANIA - First Division - Relegation Group</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Finished</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Flamurtari</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/xGXX8RTH-OSscivnC.png</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>3-1</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/vDFfHNne-I3QgPPc4.png</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Cerrik</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>26</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>ALBANIA - First Division - Relegation Group</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Finished</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Lushnja</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/Oz3NKvne-SQ3rNRbU.png</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>1-1</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/zPIZnq86-A7thZqut.png</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Elbasani</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>27</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>ALGERIA - Ligue 1</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Postponed</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Medea</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/zDPleJ6k-OnzJxC20.png</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/zFDoTHWH-WU4Aor7E.png</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>MC Alger</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>28</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>ALGERIA - Ligue 1</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Postponed</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Skikda</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/lK7xJW6k-z772ZQ0L.png</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/0Occ50UH-6kSyv7Al.png</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>CR Belouizdad</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>ENDED</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>29</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>ANGOLA - Girabola</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>16:00
+FRO</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>C.R.D. Libolo</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/pCVkxE7k-rkUKdvw4.png</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/2RrsPwCN-8zSrOQr3.png</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Ferroviario do Huambo</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>SCHEDULED</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>30</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>ANGOLA - Girabola</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>16:00
+FRO</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Onze Bravos</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/pYxgbGA6-MuTOebhA.png</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/OKDLq8VH-vswcdSPc.png</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Cuando Cubango</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>SCHEDULED</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>31</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>ANGOLA - Girabola</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>16:30
+FRO</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Baixa de Cassanje</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/hK1Xjlle-ADTx3Xx8.png</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/8dSmVoWH-bqczmqWp.png</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Sporting de Cabinda</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>SCHEDULED</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>32</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>ANGOLA - Girabola</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>16:30
+FRO</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Interclube</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/CKGpnDQq-AkaxsUG0.png</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/MkSLNJkC-xbjlUefU.png</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Petro Atletico</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>SCHEDULED</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>33</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>ANGOLA - Girabola</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>16:30
+FRO</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Sagrada</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/zL26StXH-G0VAMkIj.png</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/CIAkgfkC-8dBB3MZG.png</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Desportivo Huila</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>SCHEDULED</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>34</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>ARGENTINA - Copa de la Liga Profesional - Play Offs</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>22:30</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Estudiantes L.P.</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/buAbCpA6-IDoWSHJ3.png</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/xjDdtlT0-IHcrNFsb.png</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Independiente</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>SCHEDULED</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>35</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>ARGENTINA - Primera Nacional</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Barracas Central</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/YVxbV1iT-dtxUL4dI.png</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/IuZoU3iT-IyzpGlL0.png</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>Instituto</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>SCHEDULED</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>36</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>ARGENTINA - Primera Nacional</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>CA Estudiantes</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/I52om4Rq-C291Qktd.png</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/Sh8FTzle-bkSIR34c.png</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Quilmes</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>SCHEDULED</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>37</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>ARGENTINA - Torneo Federal</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Villa Mitre</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/A7RdPIjT-OhTmTGuP.png</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/YcnQbtVH-0Ax2tdF0.png</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Sportivo Estudiantes</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>SCHEDULED</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>38</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>ARGENTINA - Torneo Federal</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Ferro Gen. Pico</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/f9jk40VH-Mm93xzB1.png</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/x8G3nST0-dQsGvpy2.png</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Independiente Chivilcoy</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>SCHEDULED</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>39</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>ARGENTINA - Primera B - Apertura</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Flandria</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/ADxAANS0-Olw1UJbR.png</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/EHZqx0U0-4M11pKTO.png</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Justo Jose de Urquiza</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>SCHEDULED</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>40</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>ARGENTINA - Primera B - Apertura</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Canuelas</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/SQEjDG5k-jL0uhnb4.png</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/WhHN5zCN-MHtEPncg.png</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Sacachispas</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>SCHEDULED</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>41</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>ARGENTINA - Primera B - Apertura</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Comunicaciones</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/0dfSR0gT-f1B9tZqd.png</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/bkgT7zQq-rgzF3sUn.png</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>Defensores Unidos</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>SCHEDULED</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>42</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>ARGENTINA - Primera B - Apertura</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Dep. Merlo</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/UXlpx17k-WMMBgIPH.png</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/Yq5QTXhT-hSodoysk.png</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>Argentino de Quilmes</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>SCHEDULED</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>43</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>ARGENTINA - Primera B - Apertura</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>San Miguel</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/Y9U05Soe-fetYA5Qp.png</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/UqMXyZoe-pbvcVaqL.png</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>Los Andes</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>SCHEDULED</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>44</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>ARGENTINA - Primera C - Apertura</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Deportivo Espanol</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/UwNuwOU0-fuUYbJrI.png</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/rPijXYUH-fo3IhJlF.png</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>Claypole</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>SCHEDULED</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>45</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>ARGENTINA - Primera C - Apertura</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>El Porvenir</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/8lyOFqiT-QgilSLv5.png</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/EgV1HLRq-UH255ztf.png</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Laferrere</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>SCHEDULED</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>46</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>ARGENTINA - Primera C - Apertura</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Excursionistas</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/EHAE8rjC-MHtEPncg.png</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/xbwhqSA6-hSodoysk.png</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>Leandro N. Alem</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>SCHEDULED</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="n">
+        <v>47</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>ARGENTINA - Primera C - Apertura</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>San Martin Burzaco</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/dQdWpCle-29JOWySe.png</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/bwPLNP7k-EymhnHRr.png</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>Ituzaingo</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>SCHEDULED</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="n">
+        <v>48</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>ARGENTINA - Primera C - Apertura</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Sportivo Italiano</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/IFlxUwiT-AFdJu732.png</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/A31IM5CN-QV2co0EI.png</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Dock Sud</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>SCHEDULED</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="n">
+        <v>49</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>ARGENTINA - Primera D - Apertura</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Argentino de Rosario</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/b1T3r4A6-29JOWySe.png</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>https://www.flashscore.com/res/image/data/UogDzGjC-SjPVV62A.png</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>Liniers</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
         <is>
           <t>SCHEDULED</t>
         </is>

</xml_diff>

<commit_message>
Added new tables like Bundesliga, Ekstraklasa
</commit_message>
<xml_diff>
--- a/gui/mecze.xlsx
+++ b/gui/mecze.xlsx
@@ -542,7 +542,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>67  min</t>
+          <t>Finished</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -557,7 +557,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2-0</t>
+          <t>3-1</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -572,7 +572,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>LIVE</t>
+          <t>ENDED</t>
         </is>
       </c>
     </row>
@@ -1154,7 +1154,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Half Time min</t>
+          <t>65  min</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1169,7 +1169,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>1-0</t>
+          <t>2-0</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">

</xml_diff>